<commit_message>
feat: add new commands
</commit_message>
<xml_diff>
--- a/src/data/hugging.xlsx
+++ b/src/data/hugging.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAC48AF-1595-4024-8DEB-2A8085F6517F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6A66CF-F7DB-4ADD-85EE-0910F33A16F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="246">
   <si>
     <t>Label</t>
   </si>
@@ -63,13 +63,13 @@
     <t>FIND KEYWORDS</t>
   </si>
   <si>
-    <t>absorb;sink;sunk;apply;applied</t>
+    <t>absorb;sink;sunk;apply;applied;melt;melted;melts</t>
   </si>
   <si>
     <t>glide</t>
   </si>
   <si>
-    <t>makeup;foundation;concealer;primer</t>
+    <t>makeup;make up;foundation;concealer;primer</t>
   </si>
   <si>
     <t>RUN SENTIMENT ANALYSIS</t>
@@ -87,9 +87,6 @@
     <t>OTHERWISE</t>
   </si>
   <si>
-    <t>absorb (positive);absorb(negative)</t>
-  </si>
-  <si>
     <t>anti-ageing/wrinkles</t>
   </si>
   <si>
@@ -150,6 +147,423 @@
     <t>cleared skin;non-cleansing</t>
   </si>
   <si>
+    <t>congested or acne prone skin</t>
+  </si>
+  <si>
+    <t>prone;cystic;hormonal;hormonally</t>
+  </si>
+  <si>
+    <t>congest;congested;clog;clogged</t>
+  </si>
+  <si>
+    <t>acne skin (positive);acne skin (negative)</t>
+  </si>
+  <si>
+    <t>cleared pores;caused congestion</t>
+  </si>
+  <si>
+    <t>dark eye circles</t>
+  </si>
+  <si>
+    <t>eye;circles;dark;darkness;bag;hood</t>
+  </si>
+  <si>
+    <t>covered/reduced eye circles;can't cover ey circles</t>
+  </si>
+  <si>
+    <t>dewy</t>
+  </si>
+  <si>
+    <t>dewy;dewey;dew</t>
+  </si>
+  <si>
+    <t>dewy (positive);dewy (negative)</t>
+  </si>
+  <si>
+    <t>dullness</t>
+  </si>
+  <si>
+    <t>dull</t>
+  </si>
+  <si>
+    <t>less dullness;caused dullness</t>
+  </si>
+  <si>
+    <t>inflammation</t>
+  </si>
+  <si>
+    <t>inflam;inflame;inflamed</t>
+  </si>
+  <si>
+    <t>reduced inflammation;caused inflammation</t>
+  </si>
+  <si>
+    <t>as/ds/pig/disc (age spots, dark spots, discoloration, and pigmentation)</t>
+  </si>
+  <si>
+    <t>pigmentation;pigment;discolor;discolour;discoloration;dark spot;sun spot;hyper</t>
+  </si>
+  <si>
+    <t>as/ds/pig/disc (positive);as/ds/pig/disc (no change)</t>
+  </si>
+  <si>
+    <t>puffiness</t>
+  </si>
+  <si>
+    <t>puff;swollen</t>
+  </si>
+  <si>
+    <t>reduced puffiness;caused puffiness</t>
+  </si>
+  <si>
+    <t>redness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redness;red </t>
+  </si>
+  <si>
+    <t>covered/reduced redness;caused redness</t>
+  </si>
+  <si>
+    <t>scarring</t>
+  </si>
+  <si>
+    <t>scar;scars;scarring</t>
+  </si>
+  <si>
+    <t>healed scarring;no difference (scarring)</t>
+  </si>
+  <si>
+    <t>pores</t>
+  </si>
+  <si>
+    <t>shrink;shrunk;refine;refines;refined;small;smaller;reduced;size;minimise;minimising;minimize;minimized;minimised</t>
+  </si>
+  <si>
+    <t>congested;congest;clear;exfol;clean;cleans</t>
+  </si>
+  <si>
+    <t>refined pores;enlarged pores</t>
+  </si>
+  <si>
+    <t>pores (positive);pores (negative)</t>
+  </si>
+  <si>
+    <t>eczema</t>
+  </si>
+  <si>
+    <t>eczema (positive);eczema (negative)</t>
+  </si>
+  <si>
+    <t>skin tightness</t>
+  </si>
+  <si>
+    <t>firm;firmer;tight;lift;tighten;firming</t>
+  </si>
+  <si>
+    <t>firming/tightening;tightening (negative)</t>
+  </si>
+  <si>
+    <t>OPPOSITE WORDS</t>
+  </si>
+  <si>
+    <t>no;not;doesn't;does not;isn't;is not;without</t>
+  </si>
+  <si>
+    <t>CHANGE TO</t>
+  </si>
+  <si>
+    <t>non-tightening (positive)</t>
+  </si>
+  <si>
+    <t>fragrance and scent</t>
+  </si>
+  <si>
+    <t>fragran;fragranced;smel;scent</t>
+  </si>
+  <si>
+    <t>fragrance (neutral/positive);fragrance (negative/unneeded)</t>
+  </si>
+  <si>
+    <t>fragrance free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residue, white cast </t>
+  </si>
+  <si>
+    <t>sticky;cast;residue</t>
+  </si>
+  <si>
+    <t>left no residue;left residue</t>
+  </si>
+  <si>
+    <t>matte finish</t>
+  </si>
+  <si>
+    <t>matte;mattif</t>
+  </si>
+  <si>
+    <t>matte finish/feel;non-mattifying</t>
+  </si>
+  <si>
+    <t>brightening, shine, glow etc</t>
+  </si>
+  <si>
+    <t>shiny;shine;bright;glow;glowy;luminosity;lumin;sheen;radian</t>
+  </si>
+  <si>
+    <t>shine/bright/lumi/glow/rad;no glow</t>
+  </si>
+  <si>
+    <t>plumping</t>
+  </si>
+  <si>
+    <t>plump</t>
+  </si>
+  <si>
+    <t>plumping;non-plumping</t>
+  </si>
+  <si>
+    <t>nourishing and refreshing</t>
+  </si>
+  <si>
+    <t>refresh;fresh</t>
+  </si>
+  <si>
+    <t>nourish</t>
+  </si>
+  <si>
+    <t>refreshing;not refreshing</t>
+  </si>
+  <si>
+    <t>nourishing;not nourishing</t>
+  </si>
+  <si>
+    <t>nourishing/refreshing (postive);nourishing/refreshing (negative)</t>
+  </si>
+  <si>
+    <t>greasiness</t>
+  </si>
+  <si>
+    <t>oil;greas;greasy;slick</t>
+  </si>
+  <si>
+    <t>oil free finish;oily finish</t>
+  </si>
+  <si>
+    <t>consistency and texture</t>
+  </si>
+  <si>
+    <t>texture;consistency</t>
+  </si>
+  <si>
+    <t>consistency (positive);consistency (negative)</t>
+  </si>
+  <si>
+    <t>IF KEYWORDS PRESENT NO SENTIMENT</t>
+  </si>
+  <si>
+    <t>rich;creamy;foam;gel; light ;thick; thin ;liquid;mous;</t>
+  </si>
+  <si>
+    <t>IF WORDS PRESENT</t>
+  </si>
+  <si>
+    <t>soft</t>
+  </si>
+  <si>
+    <t>smooth</t>
+  </si>
+  <si>
+    <t>silky</t>
+  </si>
+  <si>
+    <t>soft texture</t>
+  </si>
+  <si>
+    <t>smooth texture</t>
+  </si>
+  <si>
+    <t>silky texture</t>
+  </si>
+  <si>
+    <t>EXCEPTION - DELETE</t>
+  </si>
+  <si>
+    <t>consistency (positive);consistency (negative</t>
+  </si>
+  <si>
+    <t>IF LABELS PRESENT</t>
+  </si>
+  <si>
+    <t>rich;creamy;foam;gel;light;thick;thin ;liquid;mous;soft texture;smooth texture;silky texture</t>
+  </si>
+  <si>
+    <t>UNLESS WORDS PRESENT</t>
+  </si>
+  <si>
+    <t>consistency;texture</t>
+  </si>
+  <si>
+    <t>dry skin and patches</t>
+  </si>
+  <si>
+    <t>dry;dry skin;dryness</t>
+  </si>
+  <si>
+    <t>drie;drying</t>
+  </si>
+  <si>
+    <t>dry skin (positive);dry skin (negative)</t>
+  </si>
+  <si>
+    <t>non-drying (positive);drying (negative)</t>
+  </si>
+  <si>
+    <t>non-drying (positive)</t>
+  </si>
+  <si>
+    <t>patch;spot;area;flakey;flake;flaky</t>
+  </si>
+  <si>
+    <t>helped dry patches</t>
+  </si>
+  <si>
+    <t>tanning</t>
+  </si>
+  <si>
+    <t>dried quickly</t>
+  </si>
+  <si>
+    <t>spots</t>
+  </si>
+  <si>
+    <t>lips</t>
+  </si>
+  <si>
+    <t>highlighted imperfections</t>
+  </si>
+  <si>
+    <t>addition of products</t>
+  </si>
+  <si>
+    <t>damaged skin</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>dark or brown skin</t>
+  </si>
+  <si>
+    <t>no changes</t>
+  </si>
+  <si>
+    <t>no difference (skin)</t>
+  </si>
+  <si>
+    <t>season of usage</t>
+  </si>
+  <si>
+    <t>summer;winter;spring;autumn;climate</t>
+  </si>
+  <si>
+    <t>season</t>
+  </si>
+  <si>
+    <t>sun protection/SPF</t>
+  </si>
+  <si>
+    <t>sun;SPF</t>
+  </si>
+  <si>
+    <t>sun damage protection</t>
+  </si>
+  <si>
+    <t>pills</t>
+  </si>
+  <si>
+    <t>pill</t>
+  </si>
+  <si>
+    <t>nightly usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> night </t>
+  </si>
+  <si>
+    <t>overnight</t>
+  </si>
+  <si>
+    <t>night</t>
+  </si>
+  <si>
+    <t>comforting, calming, soothing, and cooling</t>
+  </si>
+  <si>
+    <t>comfort</t>
+  </si>
+  <si>
+    <t>calm</t>
+  </si>
+  <si>
+    <t>cool;sooth</t>
+  </si>
+  <si>
+    <t>uncomfortable</t>
+  </si>
+  <si>
+    <t>comforting</t>
+  </si>
+  <si>
+    <t>calming</t>
+  </si>
+  <si>
+    <t>cooling/soothing</t>
+  </si>
+  <si>
+    <t>discomforting</t>
+  </si>
+  <si>
+    <t>comforting/calming</t>
+  </si>
+  <si>
+    <t>hydration/moisture</t>
+  </si>
+  <si>
+    <t>RUN SENTIMENT ANALYSIS ON WHOLE REVIEW</t>
+  </si>
+  <si>
+    <t>hydrating/moisturising;not hydrating/moisturising</t>
+  </si>
+  <si>
+    <t>supple</t>
+  </si>
+  <si>
+    <t>supple;not supple</t>
+  </si>
+  <si>
+    <t>oily skin</t>
+  </si>
+  <si>
+    <t>oily skin (positive);oily skin (negative)</t>
+  </si>
+  <si>
+    <t>combination skin (type)</t>
+  </si>
+  <si>
+    <t>IF KEYWORDS PRESENT</t>
+  </si>
+  <si>
+    <t>combo;combination</t>
+  </si>
+  <si>
+    <t>ASSIGN SENTIMENT</t>
+  </si>
+  <si>
+    <t>combination skin (positive);combination skin (negative)</t>
+  </si>
+  <si>
     <t>clear skin (type)</t>
   </si>
   <si>
@@ -159,189 +573,6 @@
     <t>clear skin (positive);clear skin (negative)</t>
   </si>
   <si>
-    <t>combination skin (type)</t>
-  </si>
-  <si>
-    <t>combo;combination</t>
-  </si>
-  <si>
-    <t>combination skin (positive);combination skin (negative)</t>
-  </si>
-  <si>
-    <t>congested or acne prone skin</t>
-  </si>
-  <si>
-    <t>prone;cystic;hormonal;hormonally</t>
-  </si>
-  <si>
-    <t>congest;congested;clog;clogged</t>
-  </si>
-  <si>
-    <t>acne skin (positive);acne skin (negative)</t>
-  </si>
-  <si>
-    <t>cleared pores;caused congestion</t>
-  </si>
-  <si>
-    <t>dark eye circles</t>
-  </si>
-  <si>
-    <t>eye;circles;dark;darkness;bag;hood</t>
-  </si>
-  <si>
-    <t>covered/reduced eye circles;can't cover ey circles</t>
-  </si>
-  <si>
-    <t>dewy</t>
-  </si>
-  <si>
-    <t>dewy;dewey;dew</t>
-  </si>
-  <si>
-    <t>dewy (positive);dewy (negative)</t>
-  </si>
-  <si>
-    <t>dullness</t>
-  </si>
-  <si>
-    <t>dull</t>
-  </si>
-  <si>
-    <t>less dullness;caused dullness</t>
-  </si>
-  <si>
-    <t>inflammation</t>
-  </si>
-  <si>
-    <t>inflam;inflame;inflamed</t>
-  </si>
-  <si>
-    <t>reduced inflammation;caused inflammation</t>
-  </si>
-  <si>
-    <t>as/ds/pig/disc (age spots, dark spots, discoloration, and pigmentation)</t>
-  </si>
-  <si>
-    <t>pigmentation;pigment;discolor;discolour;discoloration;age;dark spot;sun;spot;hyper</t>
-  </si>
-  <si>
-    <t>as/ds/pig/disc (positive);as/ds/pig/disc (no change)</t>
-  </si>
-  <si>
-    <t>puffiness</t>
-  </si>
-  <si>
-    <t>puff;swollen</t>
-  </si>
-  <si>
-    <t>reduced puffiness;caused puffiness</t>
-  </si>
-  <si>
-    <t>redness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">redness;red </t>
-  </si>
-  <si>
-    <t>covered/reduced redness;caused redness</t>
-  </si>
-  <si>
-    <t>scarring</t>
-  </si>
-  <si>
-    <t>scar;scars;scarring</t>
-  </si>
-  <si>
-    <t>healed scarring;no difference (scarring)</t>
-  </si>
-  <si>
-    <t>pores</t>
-  </si>
-  <si>
-    <t>shrink;shrunk;refine;refines;refined;small;smaller;reduced;size;minimise;minimising;minimize;minimized;minimised</t>
-  </si>
-  <si>
-    <t>congested;congest;clear;exfol;clean;cleans</t>
-  </si>
-  <si>
-    <t>refined pores;enlarged pores</t>
-  </si>
-  <si>
-    <t>pores (positive);pores (negative)</t>
-  </si>
-  <si>
-    <t>eczema</t>
-  </si>
-  <si>
-    <t>eczema (positive);eczema (negative)</t>
-  </si>
-  <si>
-    <t>skin tightness</t>
-  </si>
-  <si>
-    <t>firm;firmer;tight;lift;tighten;firming</t>
-  </si>
-  <si>
-    <t>firming/tightening;tightening (negative)</t>
-  </si>
-  <si>
-    <t>fragrance and scent</t>
-  </si>
-  <si>
-    <t>fragran;fragranced;smel;scent</t>
-  </si>
-  <si>
-    <t>fragrance (neutral/positive);fragrance (negative/unneeded)</t>
-  </si>
-  <si>
-    <t>OPPOSITE WORDS</t>
-  </si>
-  <si>
-    <t>no;not;doesn't;does not;isn't;is not;without</t>
-  </si>
-  <si>
-    <t>CHANGE TO</t>
-  </si>
-  <si>
-    <t>fragrance free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">residue, white cast </t>
-  </si>
-  <si>
-    <t>sticky;cast;residue</t>
-  </si>
-  <si>
-    <t>left no residue;left residue</t>
-  </si>
-  <si>
-    <t>matte finish</t>
-  </si>
-  <si>
-    <t>matte;mattif</t>
-  </si>
-  <si>
-    <t>matte finish/feel;non-mattifying</t>
-  </si>
-  <si>
-    <t>brightening, shine, glow etc</t>
-  </si>
-  <si>
-    <t>shiny;shine;bright;glow;glowy;luminosity;lumin;sheen;radian</t>
-  </si>
-  <si>
-    <t>shine/bright/lumi/glow/rad;no glow</t>
-  </si>
-  <si>
-    <t>plumping</t>
-  </si>
-  <si>
-    <t>plump</t>
-  </si>
-  <si>
-    <t>plumping;non-plumping</t>
-  </si>
-  <si>
     <t>normal skin (type)</t>
   </si>
   <si>
@@ -351,228 +582,9 @@
     <t>normal skin (positive);normal skin (negative)</t>
   </si>
   <si>
-    <t>nourishing and refreshing</t>
-  </si>
-  <si>
-    <t>refresh;fresh</t>
-  </si>
-  <si>
-    <t>nourish</t>
-  </si>
-  <si>
-    <t>refreshing;not refreshing</t>
-  </si>
-  <si>
-    <t>nourishing;not nourishing</t>
-  </si>
-  <si>
-    <t>nourishing/refreshing (postive);nourishing/refreshing (negative)</t>
-  </si>
-  <si>
-    <t>greasiness</t>
-  </si>
-  <si>
-    <t>oil;greas;greasy;slick</t>
-  </si>
-  <si>
-    <t>oil free finish;oily finish</t>
-  </si>
-  <si>
-    <t>consistency and texture</t>
-  </si>
-  <si>
-    <t>texture;consistency</t>
-  </si>
-  <si>
-    <t>consistency (positive);consistency (negative)</t>
-  </si>
-  <si>
-    <t>IF KEYWORDS PRESENT NO SENTIMENT</t>
-  </si>
-  <si>
-    <t>rich;creamy;foam;gel;light;thick;thin ;liquid;mous;</t>
-  </si>
-  <si>
-    <t>IF WORDS PRESENT</t>
-  </si>
-  <si>
-    <t>soft</t>
-  </si>
-  <si>
-    <t>smooth</t>
-  </si>
-  <si>
-    <t>silky</t>
-  </si>
-  <si>
-    <t>soft texture</t>
-  </si>
-  <si>
-    <t>smooth texture</t>
-  </si>
-  <si>
-    <t>silky texture</t>
-  </si>
-  <si>
-    <t>EXCEPTION - DELETE</t>
-  </si>
-  <si>
-    <t>consistency (positive);consistency (negative</t>
-  </si>
-  <si>
-    <t>IF LABELS PRESENT</t>
-  </si>
-  <si>
-    <t>rich;creamy;foam;gel;light;thick;thin ;liquid;mous;soft texture;smooth texture;silky texture</t>
-  </si>
-  <si>
-    <t>consistency;texture</t>
-  </si>
-  <si>
-    <t>dry skin and patches</t>
-  </si>
-  <si>
-    <t>dry;dry skin;dryness</t>
-  </si>
-  <si>
-    <t>drie;drying</t>
-  </si>
-  <si>
-    <t>dry skin (positive);dry skin (negative)</t>
-  </si>
-  <si>
-    <t>non-drying (positive);drying (negative)</t>
-  </si>
-  <si>
-    <t>patch;spot;area;flakey;flake;flaky</t>
-  </si>
-  <si>
-    <t>helped dry patches</t>
-  </si>
-  <si>
-    <t>tanning</t>
-  </si>
-  <si>
-    <t>dried quickly</t>
-  </si>
-  <si>
-    <t>spots</t>
-  </si>
-  <si>
-    <t>lips</t>
-  </si>
-  <si>
-    <t>highlighted imperfections</t>
-  </si>
-  <si>
-    <t>addition of products</t>
-  </si>
-  <si>
-    <t>damaged skin</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>dark or brown skin</t>
-  </si>
-  <si>
-    <t>no changes</t>
-  </si>
-  <si>
-    <t>no difference (skin)</t>
-  </si>
-  <si>
-    <t>season of usage</t>
-  </si>
-  <si>
-    <t>summer;winter;spring;autumn;climate</t>
-  </si>
-  <si>
-    <t>season</t>
-  </si>
-  <si>
-    <t>sun protection/SPF</t>
-  </si>
-  <si>
-    <t>sun;SPF</t>
-  </si>
-  <si>
-    <t>sun damage protection</t>
-  </si>
-  <si>
-    <t>pills</t>
-  </si>
-  <si>
-    <t>pill</t>
-  </si>
-  <si>
-    <t>nightly usage</t>
-  </si>
-  <si>
-    <t>night</t>
-  </si>
-  <si>
-    <t>overnight</t>
-  </si>
-  <si>
-    <t>comforting, calming, soothing, and cooling</t>
-  </si>
-  <si>
-    <t>comfort</t>
-  </si>
-  <si>
-    <t>calm</t>
-  </si>
-  <si>
-    <t>cool;sooth</t>
-  </si>
-  <si>
-    <t>uncomfortable</t>
-  </si>
-  <si>
-    <t>comforting</t>
-  </si>
-  <si>
-    <t>calming</t>
-  </si>
-  <si>
-    <t>cooling/soothing</t>
-  </si>
-  <si>
-    <t>discomforting</t>
-  </si>
-  <si>
-    <t>comforting/calming</t>
-  </si>
-  <si>
-    <t>hydration/moisture</t>
-  </si>
-  <si>
-    <t>RUN SENTIMENT ANALYSIS ON WHOLE REVIEW</t>
-  </si>
-  <si>
-    <t>hydrating/moisturising;not hydrating/moisturising</t>
-  </si>
-  <si>
-    <t>supple</t>
-  </si>
-  <si>
-    <t>supple;not supple</t>
-  </si>
-  <si>
-    <t>oily skin</t>
-  </si>
-  <si>
-    <t>oily skin (positive);oily skin (negative)</t>
-  </si>
-  <si>
     <t>pimples,breakout and acne</t>
   </si>
   <si>
-    <t>IF KEYWORDS PRESENT</t>
-  </si>
-  <si>
     <t>breakout;breakouts;broke;break</t>
   </si>
   <si>
@@ -585,9 +597,6 @@
     <t>reduce;decrease</t>
   </si>
   <si>
-    <t>ASSIGN SENTIMENT</t>
-  </si>
-  <si>
     <t>no pimples &amp; breakouts;caused pimples/breakouts</t>
   </si>
   <si>
@@ -606,7 +615,7 @@
     <t>tone and complexion</t>
   </si>
   <si>
-    <t>even ;evened;evens;evening</t>
+    <t>even;evened;evens;evening;evenness;evenly</t>
   </si>
   <si>
     <t>evened tone;evened tone (no change)</t>
@@ -636,7 +645,7 @@
     <t>irritation</t>
   </si>
   <si>
-    <t>itch</t>
+    <t xml:space="preserve"> itch</t>
   </si>
   <si>
     <t>irritat;reaction</t>
@@ -660,7 +669,7 @@
     <t>time of usage</t>
   </si>
   <si>
-    <t>day;days;second;third;fourth;repurchase</t>
+    <t>day;days;second;third;fourth;repurchase;1st;2nd;3rd;4th</t>
   </si>
   <si>
     <t>week;weeks;fortnight</t>
@@ -693,6 +702,9 @@
     <t>Breakdown regardless of category present</t>
   </si>
   <si>
+    <t>FOR THE WORD</t>
+  </si>
+  <si>
     <t>sticky;waxy;tacky</t>
   </si>
   <si>
@@ -702,13 +714,13 @@
     <t>rich</t>
   </si>
   <si>
-    <t>stinging;sting;stung;burn;tingle;tingling;tingly</t>
+    <t>stinging; sting ;stung;stings;burn;tingle;tingling;tingly</t>
   </si>
   <si>
     <t>heavy</t>
   </si>
   <si>
-    <t>light</t>
+    <t xml:space="preserve"> light </t>
   </si>
   <si>
     <t>creamy</t>
@@ -738,9 +750,6 @@
     <t>rich;not rich;heavy;non-heavy;sticky texture/residue;non-sticky texture/residue;light;creamy;non-creamy</t>
   </si>
   <si>
-    <t>FOR THE WORD</t>
-  </si>
-  <si>
     <t>pore</t>
   </si>
   <si>
@@ -753,14 +762,14 @@
     <t>EXCEPTION - CATEGORY PRESENT DON'T RUN</t>
   </si>
   <si>
-    <t>UNLESS WORDS PRESENT</t>
+    <t>CHANGE TO - OPPOSITE WORDS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,8 +802,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,6 +872,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF92D050"/>
       </patternFill>
@@ -886,7 +907,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -916,11 +937,18 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -943,6 +971,15 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -953,23 +990,42 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -978,8 +1034,14 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1197,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U46" sqref="U46"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1263,20 +1325,20 @@
       <c r="F2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="9" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>20</v>
+      <c r="K2" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="L2" s="1"/>
       <c r="N2" s="1"/>
@@ -1284,56 +1346,56 @@
     </row>
     <row r="3" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>24</v>
+      <c r="I3" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="K3" s="1"/>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>27</v>
+      <c r="C4" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>28</v>
+      <c r="E4" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>28</v>
+      <c r="G4" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="H4" s="1"/>
       <c r="J4" s="1"/>
@@ -1345,25 +1407,25 @@
     </row>
     <row r="5" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>30</v>
+      <c r="C5" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>31</v>
+      <c r="E5" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>31</v>
+      <c r="G5" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="H5" s="1"/>
       <c r="J5" s="1"/>
@@ -1372,467 +1434,476 @@
     </row>
     <row r="6" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K6" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="8" t="s">
-        <v>37</v>
+      <c r="M6" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>41</v>
+    <row r="7" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="I7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>45</v>
+      <c r="C8" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>46</v>
+      <c r="E8" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="G8" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>47</v>
+    <row r="9" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>53</v>
+      <c r="C10" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>54</v>
+      <c r="E10" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+      <c r="G10" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>56</v>
+      <c r="C11" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>57</v>
+      <c r="E11" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>57</v>
+      <c r="G11" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>60</v>
+      <c r="E12" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>62</v>
+      <c r="C13" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>63</v>
+      <c r="E13" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" ht="144" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>65</v>
+      <c r="C14" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>66</v>
+      <c r="E14" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>68</v>
+      <c r="C15" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>69</v>
+      <c r="E15" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>72</v>
+      <c r="I16" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:23" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="8" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="12" t="s">
         <v>75</v>
       </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:23" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="7" t="s">
+      <c r="G18" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="K18" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>81</v>
+      <c r="C19" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F19" s="7" t="s">
+      <c r="E19" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+      <c r="K19" s="12" t="s">
+        <v>85</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>84</v>
+      <c r="C20" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>85</v>
+      <c r="E20" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>85</v>
+      <c r="G20" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
       <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>87</v>
+      <c r="C21" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I21" s="5" t="s">
+      <c r="E21" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K21" s="9" t="s">
-        <v>88</v>
-      </c>
+      <c r="G21" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
@@ -1843,24 +1914,22 @@
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="8" t="s">
         <v>94</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="8" t="s">
         <v>95</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="12" t="s">
         <v>95</v>
       </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1873,19 +1942,19 @@
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="8" t="s">
         <v>97</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="8" t="s">
         <v>98</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="12" t="s">
         <v>98</v>
       </c>
       <c r="I23" s="1"/>
@@ -1903,264 +1972,244 @@
       <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H24" s="1"/>
+      <c r="I24" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
     <row r="25" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>103</v>
+      <c r="C25" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>104</v>
+      <c r="E25" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
+      <c r="G25" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
+      <c r="S25" s="19"/>
     </row>
     <row r="26" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>106</v>
+      <c r="C26" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>107</v>
+      <c r="E26" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="F26" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M26" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="P26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G26" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q26" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="R26" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="S26" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="U26" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="V26" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="W26" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>109</v>
+      <c r="C27" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>111</v>
+      <c r="F27" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H27" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="M27" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="O27" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="P27" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="O27" s="1"/>
+      <c r="Q27" s="12" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="28" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>116</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
       <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="S28" s="12"/>
     </row>
     <row r="29" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="N29" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="O29" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="P29" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q29" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="R29" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="S29" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="T29" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="U29" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="V29" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="W29" s="4" t="s">
-        <v>133</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
     </row>
     <row r="30" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="L30" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" s="9" t="s">
-        <v>137</v>
-      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
     <row r="31" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2179,7 +2228,7 @@
     </row>
     <row r="32" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2198,7 +2247,7 @@
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2217,7 +2266,7 @@
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2236,7 +2285,7 @@
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2255,7 +2304,7 @@
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2274,10 +2323,14 @@
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2293,14 +2346,26 @@
     </row>
     <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2312,14 +2377,26 @@
     </row>
     <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>147</v>
+      </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2331,18 +2408,26 @@
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+      <c r="F40" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>150</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -2354,25 +2439,25 @@
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>144</v>
+        <v>111</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>144</v>
+        <v>81</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>151</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G41" s="9" t="s">
-        <v>144</v>
+      <c r="G41" s="12" t="s">
+        <v>151</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -2385,88 +2470,103 @@
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="J42" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
+      <c r="K42" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="L42" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="M42" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="O42" s="1"/>
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F43" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="K43" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="L43" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
+      <c r="M43" s="12" t="s">
+        <v>166</v>
+      </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>158</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2478,104 +2578,75 @@
     </row>
     <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I45" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="J45" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="K45" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="L45" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="M45" s="4" t="s">
-        <v>162</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
     <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H46" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="I46" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="K46" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="L46" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M46" s="9" t="s">
-        <v>172</v>
-      </c>
+      <c r="C46" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C47" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
+      <c r="D47" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -2586,119 +2657,139 @@
     </row>
     <row r="48" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
+      <c r="F48" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I48" s="22"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="24"/>
+      <c r="N48" s="23"/>
       <c r="O48" s="1"/>
     </row>
     <row r="49" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
+        <v>168</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="24"/>
+      <c r="N49" s="23"/>
       <c r="O49" s="1"/>
     </row>
     <row r="50" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>182</v>
+        <v>175</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>186</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
+      </c>
+      <c r="F50" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>189</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>187</v>
+        <v>177</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="K50" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="L50" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
+      </c>
+      <c r="K50" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="L50" s="13" t="s">
+        <v>193</v>
       </c>
       <c r="M50" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N50" s="8" t="s">
-        <v>191</v>
+      <c r="N50" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="O50" s="1"/>
     </row>
     <row r="51" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="11" t="s">
-        <v>192</v>
+      <c r="A51" s="14" t="s">
+        <v>195</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>194</v>
+        <v>177</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>197</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H51" s="9" t="s">
-        <v>195</v>
+      <c r="H51" s="12" t="s">
+        <v>198</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -2710,103 +2801,103 @@
     </row>
     <row r="52" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>197</v>
+        <v>175</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>200</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>198</v>
+        <v>177</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>201</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>125</v>
+        <v>111</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="K52" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="L52" s="4" t="s">
-        <v>200</v>
+        <v>81</v>
+      </c>
+      <c r="L52" s="8" t="s">
+        <v>203</v>
       </c>
       <c r="M52" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N52" s="9" t="s">
-        <v>201</v>
+      <c r="N52" s="12" t="s">
+        <v>204</v>
       </c>
       <c r="O52" s="1"/>
     </row>
     <row r="53" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>205</v>
+        <v>177</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>208</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="I53" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J53" s="8" t="s">
-        <v>206</v>
+      <c r="J53" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="K53" s="1"/>
     </row>
     <row r="54" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>208</v>
+      <c r="C54" s="8" t="s">
+        <v>211</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>209</v>
+      <c r="E54" s="8" t="s">
+        <v>212</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G54" s="9" t="s">
-        <v>209</v>
+      <c r="G54" s="12" t="s">
+        <v>212</v>
       </c>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
@@ -2816,170 +2907,170 @@
     </row>
     <row r="55" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>217</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>215</v>
+        <v>177</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>218</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="K55" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="L55" s="10" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="K55" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="L55" s="13" t="s">
+        <v>221</v>
       </c>
       <c r="M55" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N55" s="9" t="s">
-        <v>215</v>
+      <c r="N55" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="O55" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="P55" s="16" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="56" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C56" s="4" t="s">
         <v>222</v>
       </c>
+      <c r="P55" s="26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>226</v>
+      </c>
       <c r="D56" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H56" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="I56" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J56" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="K56" s="20" t="s">
+      <c r="E56" s="25" t="s">
         <v>228</v>
       </c>
+      <c r="F56" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="G56" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H56" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="I56" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J56" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="K56" s="31" t="s">
+        <v>232</v>
+      </c>
       <c r="L56" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="M56" s="4" t="s">
-        <v>90</v>
+        <v>79</v>
+      </c>
+      <c r="M56" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="N56" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O56" s="4" t="s">
-        <v>229</v>
+      <c r="O56" s="8" t="s">
+        <v>233</v>
       </c>
       <c r="P56" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q56" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="R56" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="S56" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="T56" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="U56" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="V56" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="W56" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="X56" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y56" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z56" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA56" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="AB56" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC56" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D57" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="G57" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Q56" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="R56" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="S56" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="T56" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="U56" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="V56" s="21" t="s">
-        <v>234</v>
-      </c>
-      <c r="W56" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="X56" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y56" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z56" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AA56" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="AB56" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="AC56" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="57" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="H57" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I57" s="6" t="s">
-        <v>52</v>
+        <v>57</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
@@ -2988,12 +3079,12 @@
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
     </row>
-    <row r="58" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="16" t="s">
-        <v>221</v>
+    <row r="58" spans="1:29" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="26" t="s">
+        <v>224</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>14</v>
@@ -3001,14 +3092,14 @@
       <c r="D58" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="9" t="s">
         <v>18</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>32</v>
+        <v>244</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>

</xml_diff>